<commit_message>
ADD gb.py and btes.py
</commit_message>
<xml_diff>
--- a/inputs/ttes.xlsx
+++ b/inputs/ttes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\Documents\district_thermal_energy_systems_with_power_markets\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2960F762-F276-4409-8B22-D65894B062CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{868D3BFA-4E5A-4947-B216-3F91BB6ECDB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-1965" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2025" sheetId="1" r:id="rId1"/>
@@ -503,7 +503,7 @@
         <v>7.8630000000000004</v>
       </c>
       <c r="H2">
-        <v>5.5</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -569,7 +569,7 @@
         <v>7.8630000000000004</v>
       </c>
       <c r="H2">
-        <v>5.5</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -635,7 +635,7 @@
         <v>7.8630000000000004</v>
       </c>
       <c r="H2">
-        <v>5.5</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -701,7 +701,7 @@
         <v>7.8630000000000004</v>
       </c>
       <c r="H2">
-        <v>5.5</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -767,7 +767,7 @@
         <v>7.8630000000000004</v>
       </c>
       <c r="H2">
-        <v>5.5</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>